<commit_message>
feat: new indicators added
</commit_message>
<xml_diff>
--- a/Repo/Articulo1/output/_23a_16-07-2024.xlsx
+++ b/Repo/Articulo1/output/_23a_16-07-2024.xlsx
@@ -470,7 +470,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>07/16/24</t>
+          <t>07/23/24</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -1284,12 +1284,12 @@
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>Aceptación social</t>
+          <t>Aceptación social/Contribución a la economía local</t>
         </is>
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
-          <t>Electrificación limpia</t>
+          <t>Daño a la salud humana</t>
         </is>
       </c>
     </row>
@@ -1325,13 +1325,13 @@
         <v>0.2956878758043452</v>
       </c>
       <c r="K2" t="n">
-        <v>0.1054275896195656</v>
+        <v>0.282643134864323</v>
       </c>
       <c r="L2" t="n">
-        <v>0</v>
+        <v>0.292167395960639</v>
       </c>
       <c r="M2" t="n">
-        <v>0.2956878758043452</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -1366,13 +1366,13 @@
         <v>0.2464558444829218</v>
       </c>
       <c r="K3" t="n">
-        <v>0.1370558665054353</v>
+        <v>0.1739342368395834</v>
       </c>
       <c r="L3" t="n">
-        <v>0</v>
+        <v>0.292167395960639</v>
       </c>
       <c r="M3" t="n">
-        <v>0.2464558444829218</v>
+        <v>0.02176015267698255</v>
       </c>
     </row>
     <row r="4">
@@ -1407,13 +1407,13 @@
         <v>0.2525913679058619</v>
       </c>
       <c r="K4" t="n">
-        <v>0.1887153854190225</v>
+        <v>0.1875228490926758</v>
       </c>
       <c r="L4" t="n">
-        <v>0</v>
+        <v>0.2373860092180192</v>
       </c>
       <c r="M4" t="n">
-        <v>0.2525913679058619</v>
+        <v>0.1535298151868136</v>
       </c>
     </row>
     <row r="5">
@@ -1448,13 +1448,13 @@
         <v>0.2230225803254274</v>
       </c>
       <c r="K5" t="n">
-        <v>0.131784487024457</v>
+        <v>0.2391595756544271</v>
       </c>
       <c r="L5" t="n">
-        <v>0.1458649914978946</v>
+        <v>0.2556464714655591</v>
       </c>
       <c r="M5" t="n">
-        <v>0.2230225803254274</v>
+        <v>0.1025029910122171</v>
       </c>
     </row>
     <row r="6">
@@ -1489,13 +1489,13 @@
         <v>0.2587268913288021</v>
       </c>
       <c r="K6" t="n">
-        <v>0.2403749043326096</v>
+        <v>0.2011114613457683</v>
       </c>
       <c r="L6" t="n">
-        <v>0</v>
+        <v>0.1826046224753994</v>
       </c>
       <c r="M6" t="n">
-        <v>0.2587268913288021</v>
+        <v>0.2196154923330204</v>
       </c>
     </row>
     <row r="7">
@@ -1530,13 +1530,13 @@
         <v>0.2291581037483676</v>
       </c>
       <c r="K7" t="n">
-        <v>0.1834440059380442</v>
+        <v>0.2527481879075196</v>
       </c>
       <c r="L7" t="n">
-        <v>0.1458649914978946</v>
+        <v>0.2008650847229393</v>
       </c>
       <c r="M7" t="n">
-        <v>0.2291581037483676</v>
+        <v>0.2125119134690355</v>
       </c>
     </row>
     <row r="8">
@@ -1571,13 +1571,13 @@
         <v>0.199589316167933</v>
       </c>
       <c r="K8" t="n">
-        <v>0.1265131075434787</v>
+        <v>0.3043849144692709</v>
       </c>
       <c r="L8" t="n">
-        <v>0.2917299829957891</v>
+        <v>0.2191255469704793</v>
       </c>
       <c r="M8" t="n">
-        <v>0.199589316167933</v>
+        <v>0.08074291175723833</v>
       </c>
     </row>
     <row r="9">
@@ -1612,13 +1612,13 @@
         <v>0.2279753522451502</v>
       </c>
       <c r="K9" t="n">
-        <v>0.2045295238619573</v>
+        <v>0.133168400080306</v>
       </c>
       <c r="L9" t="n">
-        <v>0</v>
+        <v>0.2373860092180192</v>
       </c>
       <c r="M9" t="n">
-        <v>0.2279753522451502</v>
+        <v>0.1535298151868136</v>
       </c>
     </row>
     <row r="10">
@@ -1653,13 +1653,13 @@
         <v>0.1984065646647157</v>
       </c>
       <c r="K10" t="n">
-        <v>0.1475986254673919</v>
+        <v>0.1848051266420573</v>
       </c>
       <c r="L10" t="n">
-        <v>0.1458649914978946</v>
+        <v>0.2556464714655591</v>
       </c>
       <c r="M10" t="n">
-        <v>0.1984065646647157</v>
+        <v>0.1025029910122171</v>
       </c>
     </row>
     <row r="11">
@@ -1694,13 +1694,13 @@
         <v>0.2341108756680903</v>
       </c>
       <c r="K11" t="n">
-        <v>0.2561890427755445</v>
+        <v>0.1467570123333985</v>
       </c>
       <c r="L11" t="n">
-        <v>0</v>
+        <v>0.1826046224753994</v>
       </c>
       <c r="M11" t="n">
-        <v>0.2341108756680903</v>
+        <v>0.2413763058080368</v>
       </c>
     </row>
     <row r="12">
@@ -1735,13 +1735,13 @@
         <v>0.2045420880876558</v>
       </c>
       <c r="K12" t="n">
-        <v>0.199258144380979</v>
+        <v>0.1983937388951498</v>
       </c>
       <c r="L12" t="n">
-        <v>0.1458649914978946</v>
+        <v>0.2008650847229393</v>
       </c>
       <c r="M12" t="n">
-        <v>0.2045420880876558</v>
+        <v>0.2342719927240143</v>
       </c>
     </row>
     <row r="13">
@@ -1776,13 +1776,13 @@
         <v>0.1749733005072213</v>
       </c>
       <c r="K13" t="n">
-        <v>0.1423272459864136</v>
+        <v>0.2500304654569011</v>
       </c>
       <c r="L13" t="n">
-        <v>0.2917299829957891</v>
+        <v>0.2191255469704793</v>
       </c>
       <c r="M13" t="n">
-        <v>0.1749733005072213</v>
+        <v>0.1025029910122171</v>
       </c>
     </row>
     <row r="14">
@@ -1817,13 +1817,13 @@
         <v>0.210677611510596</v>
       </c>
       <c r="K14" t="n">
-        <v>0.2509176632945662</v>
+        <v>0.2119823511482422</v>
       </c>
       <c r="L14" t="n">
-        <v>0.1458649914978946</v>
+        <v>0.1460836979803195</v>
       </c>
       <c r="M14" t="n">
-        <v>0.210677611510596</v>
+        <v>0.3003584040902587</v>
       </c>
     </row>
     <row r="15">
@@ -1858,13 +1858,13 @@
         <v>0.1811088239301615</v>
       </c>
       <c r="K15" t="n">
-        <v>0.1939867649000008</v>
+        <v>0.2636190777099935</v>
       </c>
       <c r="L15" t="n">
-        <v>0.2917299829957891</v>
+        <v>0.1643441602278594</v>
       </c>
       <c r="M15" t="n">
-        <v>0.1811088239301615</v>
+        <v>0.2125119134690355</v>
       </c>
     </row>
     <row r="16">
@@ -1899,13 +1899,13 @@
         <v>0.1972238131614983</v>
       </c>
       <c r="K16" t="n">
-        <v>0.168684143391305</v>
+        <v>0.06522533881484376</v>
       </c>
       <c r="L16" t="n">
-        <v>0</v>
+        <v>0.292167395960639</v>
       </c>
       <c r="M16" t="n">
-        <v>0.1972238131614983</v>
+        <v>0.02176015267698255</v>
       </c>
     </row>
     <row r="17">
@@ -1940,13 +1940,13 @@
         <v>0.2094948600073786</v>
       </c>
       <c r="K17" t="n">
-        <v>0.2720031812184793</v>
+        <v>0.09240256332102866</v>
       </c>
       <c r="L17" t="n">
-        <v>0</v>
+        <v>0.1826046224753994</v>
       </c>
       <c r="M17" t="n">
-        <v>0.2094948600073786</v>
+        <v>0.2413763058080368</v>
       </c>
     </row>
     <row r="18">
@@ -1981,13 +1981,13 @@
         <v>0.1799260724269441</v>
       </c>
       <c r="K18" t="n">
-        <v>0.2150722828239139</v>
+        <v>0.14403928988278</v>
       </c>
       <c r="L18" t="n">
-        <v>0.1458649914978946</v>
+        <v>0.2008650847229393</v>
       </c>
       <c r="M18" t="n">
-        <v>0.1799260724269441</v>
+        <v>0.2342719927240143</v>
       </c>
     </row>
     <row r="19">
@@ -2022,13 +2022,13 @@
         <v>0.1503572848465095</v>
       </c>
       <c r="K19" t="n">
-        <v>0.1581413844293484</v>
+        <v>0.1956760164445313</v>
       </c>
       <c r="L19" t="n">
-        <v>0.2917299829957891</v>
+        <v>0.2191255469704793</v>
       </c>
       <c r="M19" t="n">
-        <v>0.1503572848465095</v>
+        <v>0.1025029910122171</v>
       </c>
     </row>
     <row r="20">
@@ -2063,13 +2063,13 @@
         <v>0.1860615958498842</v>
       </c>
       <c r="K20" t="n">
-        <v>0.2667318017375011</v>
+        <v>0.1576279021358724</v>
       </c>
       <c r="L20" t="n">
-        <v>0.1458649914978946</v>
+        <v>0.1460836979803195</v>
       </c>
       <c r="M20" t="n">
-        <v>0.1860615958498842</v>
+        <v>0.3221184833452375</v>
       </c>
     </row>
     <row r="21">
@@ -2104,13 +2104,13 @@
         <v>0.1564928082694497</v>
       </c>
       <c r="K21" t="n">
-        <v>0.2098009033429356</v>
+        <v>0.2092646286976237</v>
       </c>
       <c r="L21" t="n">
-        <v>0.2917299829957891</v>
+        <v>0.1643441602278594</v>
       </c>
       <c r="M21" t="n">
-        <v>0.1564928082694497</v>
+        <v>0.2342719927240143</v>
       </c>
     </row>
     <row r="22">
@@ -2145,13 +2145,13 @@
         <v>0.2217659068532589</v>
       </c>
       <c r="K22" t="n">
-        <v>0.3753222190456537</v>
+        <v>0.1195797878272136</v>
       </c>
       <c r="L22" t="n">
-        <v>0</v>
+        <v>0.07304184899015975</v>
       </c>
       <c r="M22" t="n">
-        <v>0.2217659068532589</v>
+        <v>0.4392317188860784</v>
       </c>
     </row>
     <row r="23">
@@ -2186,13 +2186,13 @@
         <v>0.1626283316923899</v>
       </c>
       <c r="K23" t="n">
-        <v>0.2614604222565228</v>
+        <v>0.2228532409507162</v>
       </c>
       <c r="L23" t="n">
-        <v>0.2917299829957891</v>
+        <v>0.1095627734852396</v>
       </c>
       <c r="M23" t="n">
-        <v>0.1626283316923899</v>
+        <v>0.3003584040902587</v>
       </c>
     </row>
     <row r="24">
@@ -2227,13 +2227,13 @@
         <v>0.1034907565315208</v>
       </c>
       <c r="K24" t="n">
-        <v>0.1475986254673919</v>
+        <v>0.3261266940742188</v>
       </c>
       <c r="L24" t="n">
-        <v>0.5834599659915782</v>
+        <v>0.1460836979803195</v>
       </c>
       <c r="M24" t="n">
-        <v>0.1034907565315208</v>
+        <v>0.08074291175723833</v>
       </c>
     </row>
   </sheetData>
@@ -2384,186 +2384,186 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>0.6962435973600611</v>
+        <v>0.7530530141799295</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="B3" t="n">
-        <v>0.4834877150700716</v>
+        <v>0.7217855148090941</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="B4" t="n">
-        <v>0.4803564314019066</v>
+        <v>0.7210686234971996</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>0.4796111155994668</v>
+        <v>0.6860518801332826</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="B6" t="n">
-        <v>0.4688590157211237</v>
+        <v>0.6821010285108894</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B7" t="n">
-        <v>0.4681564847721486</v>
+        <v>0.6736130465966271</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="B8" t="n">
-        <v>0.4559834350965712</v>
+        <v>0.6670106954526674</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="B9" t="n">
-        <v>0.3180294904538975</v>
+        <v>0.6633767066819743</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B10" t="n">
-        <v>0.3168710410686629</v>
+        <v>0.6582670122009904</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B11" t="n">
-        <v>0.306423025290815</v>
+        <v>0.5885289903265453</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="B12" t="n">
-        <v>0.3042593424529688</v>
+        <v>0.5713649193293828</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B13" t="n">
-        <v>0.2995947405354777</v>
+        <v>0.5206271658452135</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="B14" t="n">
-        <v>0.2877706852117689</v>
+        <v>0.5073357613457374</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="B15" t="n">
-        <v>0.2837758386085641</v>
+        <v>0.4790585469410924</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="B16" t="n">
-        <v>0.2756508973173974</v>
+        <v>0.4733654728337816</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B17" t="n">
-        <v>0.2649217944273705</v>
+        <v>0.4582814329096751</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="B18" t="n">
-        <v>0.2504357177297277</v>
+        <v>0.4552435577376918</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="B19" t="n">
-        <v>0.2331076723845173</v>
+        <v>0.4339811154156679</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="B20" t="n">
-        <v>0.2307956761944421</v>
+        <v>0.4180925665283239</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B21" t="n">
-        <v>0.2296904521895157</v>
+        <v>0.3538192547620688</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="B22" t="n">
-        <v>0.2125213251616612</v>
+        <v>0.3439000330375241</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="B23" t="n">
-        <v>0.2099293750627683</v>
+        <v>0.304685973317776</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="B24" t="n">
-        <v>0.172615744804787</v>
+        <v>0.1872750736235602</v>
       </c>
     </row>
   </sheetData>

</xml_diff>